<commit_message>
Working Copy of the code
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smit.rathore\Documents\UiPath\igo-training-wi4-performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0969E6F-0BEF-456F-9C96-6F5D8D61CF17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFA26ED-5825-488F-A854-449CB58F6DFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37236" yWindow="4044" windowWidth="19200" windowHeight="10056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>ACME_CREDENTIALS_IGO</t>
   </si>
   <si>
-    <t>igo-training-wi4_test</t>
+    <t>igo-training-wi4</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>